<commit_message>
update kế hoạch làm việc
</commit_message>
<xml_diff>
--- a/doc/KLTNHK2_20182019_09_KE-HOACH-THUC-HIEN-SV_NguyenVietHoang_NguyenDucHieuAn.xlsx
+++ b/doc/KLTNHK2_20182019_09_KE-HOACH-THUC-HIEN-SV_NguyenVietHoang_NguyenDucHieuAn.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="136">
   <si>
     <t>KẾ HOẠCH THỰC HIỆN KHÓA LUẬN TỐT NGHIỆP</t>
   </si>
@@ -281,18 +281,6 @@
 - Tham khảo trang web nội bộ của Fsoft
 - Tìm hiểu các UML Diagram
 - Học các quy định về bảo mật của công ty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Củng cố kiến thức Spring Boot (Controller, Service, Repository, Interceptor, Configure)
-- Củng cố kiến thức Hibernate: các quan hệ entities(OneToOne, OneToMany,ManyToMany), các cấu trúc query
-- MySql(ưu nhược điểm so với SQL Server), cách cấu hình, cài đặt MySql (tài liệu Fsoft cung cấp, google)
-- Tìm hiểu Docker là gì? Tại sao phải sử dụng Docker và cách cấu hình Docker.
-- Demo code mẫu cho phần Spring Boot sứ dụng Hibernate thao tác CRUD với MySql
-- Viết User stories với các actor:
-+ Nhân viên (Quản lý kỹ năng CV, Tìm kiếm cơ bản, Đánh giá, Hướng dẫn sử dụng.
-+ Quản lý(Tìm kiếm nâng cao,Đánh giá, Xem đánh giá).
-+ Nhân sự (Tìm kiếm nâng cao, Xác nhận CV, Cập nhật thông tin nhân viên, Phân tích dữ liệu mạng xã hội của nhân viên).
-</t>
   </si>
   <si>
     <t>23/01/2019</t>
@@ -308,24 +296,6 @@
 + Màn hình tìm kiếm, gợi ý.
 + Màn hình phân tích dữ liệu mạng xã hội.
 - Code demo phần tính năng về chứng chỉ </t>
-  </si>
-  <si>
-    <t>- Thiết kế Usecase.
-- Thiết kế Sitemap.
-- Thiết kế Entity diagram.
-- Thiết kế Class diagram.
-- Vẽ sequence chức năng Quản lý Certificate.</t>
-  </si>
-  <si>
-    <t>- Chỉnh sửa lại Thiết kế Usecase, đặc tả,  Sitemap, Entity, Activity, Sequency, Class diagram.
-- Tiến hành code back-end (rest api) cho các tính năng căn bản như thêm, xoá, sửa các kỹ năng kỹ thuât, ngoại ngữ của nhân viên.
-- Tiến hành code front-end các component cho chức năng thêm, xóa sửa kỹ năng kỹ thuật, ngoại ngữ.</t>
-  </si>
-  <si>
-    <t>- Chỉnh sửa lại Thiết kế Usecase, đặc tả,  Sitemap, Entity, Activity, Sequency, Class diagram.
-- Chỉnh sửa code back-end (rest api) cho các tính năng căn bản như thêm, xoá, sửa các kỹ năng, ngoại ngữ, chứng chỉ, bằng cấp, kinh nghiệm làm việc của nhân viên.
-- Chỉnh sửa code front-end các component cho chức năng thêm, xóa sửa kỹ năng kỹ thuật, ngoại ngữ.
-- Thiết kế một số Test Case và Unit Test cho các tính năng trên.</t>
   </si>
   <si>
     <t>13/05/2019</t>
@@ -489,24 +459,6 @@
     </r>
   </si>
   <si>
-    <t>- Tạo component xem nhật ký thay đổi dữ liệu.
-- Phân quyền ứng dụng
-- Viết thuật toán tìm kiếm sắp xếp ứng viên cho dự án.</t>
-  </si>
-  <si>
-    <t>- Thiết kế các màn hình cho nhân viên nhân sự.
-- Tạo api tính năng duyệt cv cho nhân sự, thống kê, quản lý dữ liệu, thống kê nhân viên.
-- Tạo các component Angular thống kê, quản lý dữ liệu.
-- Chỉnh sửa Sequence và Class diagram.
-- Viết tài liệu kiến thức nền tảng, tổng quan, mục tiêu của đồ án.</t>
-  </si>
-  <si>
-    <t>- Thiết kế màn hình quản lý dữ liệu của hệ thống bằng handson table.
-- Tạo API cho chức năng quản lý dữ liệu bằng handson table.
-- Thiết kế màn hình tìm kiếm nâng cao cho nhân viên nhân sự.
-- Tạo API cho việc tìm kiếm nâng cao của nhân viên nhân sự.</t>
-  </si>
-  <si>
     <t>- Test các tính năng và fix lỗi API và Angular</t>
   </si>
   <si>
@@ -515,6 +467,97 @@
 - Tạo các component Angular thống kê, quản lý dữ liệu.
 - Chỉnh sửa Sequence và Class diagram
 - Viết tài liệu kiến thức nền tảng, tổng quan, mục tiêu của đồ án.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Củng cố kiến thức Spring Boot (Controller, Service, Repository, Interceptor, Configure)
+- Củng cố kiến thức Hibernate: các quan hệ entities(OneToOne, OneToMany,ManyToMany), các cấu trúc query
+- MySql(ưu nhược điểm so với SQL Server), cách cấu hình, cài đặt MySql (tài liệu Fsoft cung cấp, google)
+- Tìm hiểu Docker là gì? Tại sao phải sử dụng Docker và cách cấu hình Docker.
+- Demo code mẫu cho phần Spring Boot sứ dụng Hibernate thao tác CRUD với MySql
+- Viết User stories với các actor:
++ Nhân viên (Quản lý kỹ năng CV, Tìm kiếm cơ bản, Đánh giá, Hướng dẫn sử dụng.
++ Quản lý(Tìm kiếm nâng cao, Đánh giá, Xem đánh giá).
++ Nhân sự (Tìm kiếm nâng cao, Xác nhận CV, Cập nhật thông tin nhân viên, Phân tích dữ liệu mạng xã hội của nhân viên).
+</t>
+  </si>
+  <si>
+    <t>- Chỉnh sửa tài liệu và gặp giảng viên phản biện.</t>
+  </si>
+  <si>
+    <t>20/05/2019</t>
+  </si>
+  <si>
+    <t>26/05/2019</t>
+  </si>
+  <si>
+    <t>- Kiểm thử các chức năng, sửa lỗi API và Angular.
+- Chỉnh responsive cho hệ thống.
+- Chỉnh sửa nội dung tài liệu: phần lý thuyết, mô tả chức năng của hệ thống.</t>
+  </si>
+  <si>
+    <t>- Thiết kế các màn hình cho nhân viên nhân sự.
+- Tạo API tính năng cập nhật trạng thái hồ sơ của nhân viên, thống kê, quản lý dữ liệu, thống kê nhân viên.
+- Tạo các component Angular thống kê, quản lý dữ liệu.
+- Chỉnh sửa Sequence và Class diagram.
+- Viết tài liệu kiến thức nền tảng, tổng quan, mục tiêu của đồ án.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Chỉnh sửa lại Thiết kế Usecase, đặc tả, Entity diagram, Activity diagram, Sequence diagram, Class diagram, mô hình cơ sở dữ liệu quan hệ.
+- Tiến hành code back-end (RESTful API) cho các tính năng căn bản như thêm, xoá, sửa các kỹ năng kỹ thuât, ngoại ngữ của nhân viên.
+- Tiến hành code front-end các component cho chức năng thêm, xóa sửa kỹ năng kỹ thuật, ngoại ngữ.</t>
+  </si>
+  <si>
+    <t>- Chỉnh sửa lại Thiết kế Usecase, đặc tả, Entity diagram, Activity, Sequency, Class diagram.
+- Chỉnh sửa code back-end (RESTful API) cho các tính năng căn bản như thêm, xoá, sửa các kỹ năng, ngoại ngữ, chứng chỉ, bằng cấp, kinh nghiệm làm việc của nhân viên.
+- Chỉnh sửa code front-end các component cho chức năng thêm, xóa sửa kỹ năng kỹ thuật, ngoại ngữ.
+- Thiết kế một số Test Case và Unit Test cho các tính năng trên.</t>
+  </si>
+  <si>
+    <t>- Tạo component trang hồ sơ của nhân viên.
+- Tạo component xem nhật ký thay đổi dữ liệu.
+- Cấu hình phân quyền cho hệ thống.
+- Viết thuật toán tìm kiếm sắp xếp ứng viên cho dự án.
+- Tạo API lưu, xem nhật ký thay đổi.
+- Deploy phiên bản code v0.2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Tạo API cho nhập, xuất dữ liệu nhân viên, tính năng hỗ trợ nhân viên.
+- Tích hợp xác thực tài khoản với hệ thống CAS
+- Tạo Angular Component cho nhập dữ liệu nhân viên mô phỏng dạng bảng tính (spreadsheet).
+- Deploy phiên bản code v0.1.
+</t>
+  </si>
+  <si>
+    <t>- Chỉnh sửa tài liệu và gặp giảng viên phản biện.
+- Deploy phiên bản code v0.4.</t>
+  </si>
+  <si>
+    <t>- Cập nhật thuật toán gợi ý tìm kiếm các ứng viên phù hợp với các tiêu chí yêu cầu của dự án.
+- Chỉnh sửa component quản lý dự án.
+- Chỉnh sửa API cập nhật trạng thái của dự án, thêm logic ràng buộc dữ liệu khi cập nhật trạng thái của dự án.
+- Tạo component tìm kiếm cho nhân viên nhân sự.
+- Deploy phiên bản code v0.3.</t>
+  </si>
+  <si>
+    <t>- Thiết kế Usecase tổng quát, đặc tả chi tiết usecase.
+- Thiết kế Entity diagram.
+- Thiết kế Class diagram.
+- Vẽ sequence chức năng Quản lý Certificate.
+- Cập nhật User stories:
+    + Nhân viên: hủy chức năng đánh giá và tìm kiếm.
+    + Nhân viên nhân sự: hủy chức năng phân tích mạng xã hội, thêm chức năng thống kê, thêm chức năng xem nhật ký thay dổi của nhân viên, thêm chức năng quản lý dữ liệu của hệ thống.
+    + Nhân viên quản lý dự án: hủy chức năng đánh giá, thêm chức năng quản lý thông tin dự án, thêm chức năng gợi ý ứng viên phù hợp cho vị trí trong dự án, thêm chức năng tìm kiếm nhân viên.</t>
+  </si>
+  <si>
+    <t>- Thiết kế các màn hình của nhân viên quản lý.
+- Tạo API cho chức năng của nhân viên quản lý dự án: quản lý dự án, quản lý vị trí trong dự án, gợi ý tìm kiếm ứng viên cho dự án.
+- Tạo comonent Angular cho quản lý dự án, vị trí trong dự án và tìm kiếm ứng viên.</t>
+  </si>
+  <si>
+    <t>- Thiết kế màn hình quản lý dữ liệu của hệ thống bằng bảng tính.
+- Tạo API cho chức năng quản lý dữ liệu bằng bảng tính.
+- Thiết kế màn hình tìm kiếm nâng cao cho nhân viên nhân sự.
+- Tạo API cho việc tìm kiếm nâng cao của nhân viên nhân sự.</t>
   </si>
 </sst>
 </file>
@@ -761,7 +804,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -867,11 +910,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1068,9 +1120,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="32" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1102,6 +1151,15 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2315,8 +2373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2330,12 +2388,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="66.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -2642,7 +2700,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="57" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>13</v>
@@ -3002,7 +3060,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="57" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>41</v>
@@ -3074,7 +3132,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="57" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>46</v>
@@ -3110,7 +3168,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="57" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>48</v>
@@ -4236,10 +4294,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4255,14 +4313,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
       <c r="G1" s="20"/>
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
@@ -4457,7 +4515,7 @@
       <c r="D7" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="66" t="s">
+      <c r="E7" s="83" t="s">
         <v>69</v>
       </c>
       <c r="F7" s="67" t="s">
@@ -4484,7 +4542,7 @@
       <c r="Y7" s="25"/>
       <c r="Z7" s="25"/>
     </row>
-    <row r="8" spans="1:26" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="68">
         <v>1</v>
       </c>
@@ -4497,10 +4555,10 @@
       <c r="D8" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="71" t="s">
+      <c r="E8" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="72"/>
+      <c r="F8" s="71"/>
       <c r="G8" s="26"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
@@ -4522,11 +4580,11 @@
       <c r="Y8" s="21"/>
       <c r="Z8" s="21"/>
     </row>
-    <row r="9" spans="1:26" ht="240" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="208.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="68">
         <v>2</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="72" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="69" t="s">
@@ -4535,10 +4593,10 @@
       <c r="D9" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="71" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="72"/>
+      <c r="E9" s="75" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="71"/>
       <c r="G9" s="26"/>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
@@ -4560,23 +4618,23 @@
       <c r="Y9" s="21"/>
       <c r="Z9" s="21"/>
     </row>
-    <row r="10" spans="1:26" ht="174.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="171.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="68">
         <v>3</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="72" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="69" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="74" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="72"/>
+      <c r="F10" s="71"/>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
@@ -4598,11 +4656,11 @@
       <c r="Y10" s="21"/>
       <c r="Z10" s="21"/>
     </row>
-    <row r="11" spans="1:26" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="68">
         <v>4</v>
       </c>
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="72" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="69" t="s">
@@ -4611,10 +4669,10 @@
       <c r="D11" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="74" t="s">
+      <c r="E11" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="72"/>
+      <c r="F11" s="71"/>
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
@@ -4636,11 +4694,11 @@
       <c r="Y11" s="21"/>
       <c r="Z11" s="21"/>
     </row>
-    <row r="12" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="68">
         <v>5</v>
       </c>
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="72" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="69" t="s">
@@ -4649,10 +4707,10 @@
       <c r="D12" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="74" t="s">
+      <c r="E12" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="72"/>
+      <c r="F12" s="71"/>
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
@@ -4674,11 +4732,11 @@
       <c r="Y12" s="21"/>
       <c r="Z12" s="21"/>
     </row>
-    <row r="13" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="68">
         <v>6</v>
       </c>
-      <c r="B13" s="73" t="s">
+      <c r="B13" s="72" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="69" t="s">
@@ -4687,10 +4745,10 @@
       <c r="D13" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="74" t="s">
+      <c r="E13" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="72"/>
+      <c r="F13" s="71"/>
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
@@ -4712,21 +4770,23 @@
       <c r="Y13" s="21"/>
       <c r="Z13" s="21"/>
     </row>
-    <row r="14" spans="1:26" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="68">
         <v>7</v>
       </c>
-      <c r="B14" s="73" t="s">
+      <c r="B14" s="72" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="69"/>
+      <c r="D14" s="69" t="s">
+        <v>28</v>
+      </c>
       <c r="E14" s="74" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="72"/>
+        <v>133</v>
+      </c>
+      <c r="F14" s="71"/>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
@@ -4748,21 +4808,23 @@
       <c r="Y14" s="21"/>
       <c r="Z14" s="21"/>
     </row>
-    <row r="15" spans="1:26" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="68">
         <v>8</v>
       </c>
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="72" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="69"/>
+      <c r="D15" s="69" t="s">
+        <v>31</v>
+      </c>
       <c r="E15" s="74" t="s">
-        <v>76</v>
-      </c>
-      <c r="F15" s="72"/>
+        <v>127</v>
+      </c>
+      <c r="F15" s="71"/>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
@@ -4788,17 +4850,19 @@
       <c r="A16" s="68">
         <v>9</v>
       </c>
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="72" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="69"/>
-      <c r="E16" s="75" t="s">
-        <v>77</v>
-      </c>
-      <c r="F16" s="72"/>
+      <c r="D16" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="74" t="s">
+        <v>128</v>
+      </c>
+      <c r="F16" s="71"/>
       <c r="G16" s="21"/>
       <c r="H16" s="21"/>
       <c r="I16" s="21"/>
@@ -4820,11 +4884,11 @@
       <c r="Y16" s="21"/>
       <c r="Z16" s="21"/>
     </row>
-    <row r="17" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="68">
         <v>10</v>
       </c>
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="72" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="69" t="s">
@@ -4833,10 +4897,10 @@
       <c r="D17" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="75" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="72"/>
+      <c r="E17" s="74" t="s">
+        <v>130</v>
+      </c>
+      <c r="F17" s="71"/>
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
       <c r="I17" s="21"/>
@@ -4858,11 +4922,11 @@
       <c r="Y17" s="21"/>
       <c r="Z17" s="21"/>
     </row>
-    <row r="18" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="68">
         <v>11</v>
       </c>
-      <c r="B18" s="73" t="s">
+      <c r="B18" s="72" t="s">
         <v>39</v>
       </c>
       <c r="C18" s="69" t="s">
@@ -4871,10 +4935,10 @@
       <c r="D18" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="75" t="s">
+      <c r="E18" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="72"/>
+      <c r="F18" s="71"/>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
@@ -4896,11 +4960,11 @@
       <c r="Y18" s="21"/>
       <c r="Z18" s="21"/>
     </row>
-    <row r="19" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="68">
         <v>12</v>
       </c>
-      <c r="B19" s="73" t="s">
+      <c r="B19" s="72" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="69" t="s">
@@ -4909,10 +4973,10 @@
       <c r="D19" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="75" t="s">
-        <v>123</v>
-      </c>
-      <c r="F19" s="72"/>
+      <c r="E19" s="74" t="s">
+        <v>129</v>
+      </c>
+      <c r="F19" s="71"/>
       <c r="G19" s="21"/>
       <c r="H19" s="21"/>
       <c r="I19" s="21"/>
@@ -4934,11 +4998,11 @@
       <c r="Y19" s="21"/>
       <c r="Z19" s="21"/>
     </row>
-    <row r="20" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="68">
         <v>13</v>
       </c>
-      <c r="B20" s="73" t="s">
+      <c r="B20" s="72" t="s">
         <v>44</v>
       </c>
       <c r="C20" s="69" t="s">
@@ -4947,10 +5011,10 @@
       <c r="D20" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="75" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" s="72"/>
+      <c r="E20" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="F20" s="71"/>
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
       <c r="I20" s="21"/>
@@ -4972,11 +5036,11 @@
       <c r="Y20" s="21"/>
       <c r="Z20" s="21"/>
     </row>
-    <row r="21" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="68">
         <v>14</v>
       </c>
-      <c r="B21" s="73" t="s">
+      <c r="B21" s="72" t="s">
         <v>46</v>
       </c>
       <c r="C21" s="69" t="s">
@@ -4985,10 +5049,10 @@
       <c r="D21" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="75" t="s">
-        <v>124</v>
-      </c>
-      <c r="F21" s="72"/>
+      <c r="E21" s="82" t="s">
+        <v>132</v>
+      </c>
+      <c r="F21" s="71"/>
       <c r="G21" s="21"/>
       <c r="H21" s="21"/>
       <c r="I21" s="21"/>
@@ -5010,11 +5074,11 @@
       <c r="Y21" s="21"/>
       <c r="Z21" s="21"/>
     </row>
-    <row r="22" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="68">
         <v>15</v>
       </c>
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="72" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="69" t="s">
@@ -5023,10 +5087,10 @@
       <c r="D22" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="76" t="s">
-        <v>125</v>
-      </c>
-      <c r="F22" s="72"/>
+      <c r="E22" s="74" t="s">
+        <v>126</v>
+      </c>
+      <c r="F22" s="71"/>
       <c r="G22" s="21"/>
       <c r="H22" s="21"/>
       <c r="I22" s="21"/>
@@ -5048,11 +5112,11 @@
       <c r="Y22" s="21"/>
       <c r="Z22" s="21"/>
     </row>
-    <row r="23" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="68">
         <v>16</v>
       </c>
-      <c r="B23" s="73" t="s">
+      <c r="B23" s="72" t="s">
         <v>51</v>
       </c>
       <c r="C23" s="69" t="s">
@@ -5061,10 +5125,10 @@
       <c r="D23" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="76" t="s">
-        <v>126</v>
-      </c>
-      <c r="F23" s="72"/>
+      <c r="E23" s="75" t="s">
+        <v>135</v>
+      </c>
+      <c r="F23" s="71"/>
       <c r="G23" s="21"/>
       <c r="H23" s="21"/>
       <c r="I23" s="21"/>
@@ -5086,11 +5150,11 @@
       <c r="Y23" s="21"/>
       <c r="Z23" s="21"/>
     </row>
-    <row r="24" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="68">
         <v>17</v>
       </c>
-      <c r="B24" s="73" t="s">
+      <c r="B24" s="72" t="s">
         <v>53</v>
       </c>
       <c r="C24" s="69" t="s">
@@ -5099,10 +5163,10 @@
       <c r="D24" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="76" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="72"/>
+      <c r="E24" s="75" t="s">
+        <v>125</v>
+      </c>
+      <c r="F24" s="71"/>
       <c r="G24" s="21"/>
       <c r="H24" s="21"/>
       <c r="I24" s="21"/>
@@ -5124,11 +5188,11 @@
       <c r="Y24" s="21"/>
       <c r="Z24" s="21"/>
     </row>
-    <row r="25" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="68">
         <v>18</v>
       </c>
-      <c r="B25" s="73" t="s">
+      <c r="B25" s="72" t="s">
         <v>55</v>
       </c>
       <c r="C25" s="69" t="s">
@@ -5137,10 +5201,10 @@
       <c r="D25" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="76" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" s="72"/>
+      <c r="E25" s="75" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" s="71"/>
       <c r="G25" s="21"/>
       <c r="H25" s="21"/>
       <c r="I25" s="21"/>
@@ -5162,23 +5226,23 @@
       <c r="Y25" s="21"/>
       <c r="Z25" s="21"/>
     </row>
-    <row r="26" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="68">
         <v>19</v>
       </c>
-      <c r="B26" s="73" t="s">
-        <v>78</v>
+      <c r="B26" s="72" t="s">
+        <v>74</v>
       </c>
       <c r="C26" s="69" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D26" s="69" t="s">
-        <v>79</v>
-      </c>
-      <c r="E26" s="76" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" s="72"/>
+        <v>75</v>
+      </c>
+      <c r="E26" s="75" t="s">
+        <v>131</v>
+      </c>
+      <c r="F26" s="71"/>
       <c r="G26" s="21"/>
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
@@ -5200,7 +5264,24 @@
       <c r="Y26" s="21"/>
       <c r="Z26" s="21"/>
     </row>
-    <row r="27" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="68">
+        <v>20</v>
+      </c>
+      <c r="B27" s="72" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" s="69" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="69" t="s">
+        <v>124</v>
+      </c>
+      <c r="E27" s="75" t="s">
+        <v>122</v>
+      </c>
+      <c r="F27" s="71"/>
+    </row>
     <row r="28" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5398,8 +5479,8 @@
     <row r="222" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="223" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="224" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6172,8 +6253,6 @@
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
@@ -6257,14 +6336,14 @@
     </row>
     <row r="2" spans="1:116" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="79" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
+      <c r="B2" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
       <c r="H2" s="28"/>
       <c r="I2" s="28"/>
       <c r="J2" s="28"/>
@@ -6305,14 +6384,14 @@
     </row>
     <row r="3" spans="1:116" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
       <c r="H3" s="30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I3" s="30"/>
       <c r="J3" s="30"/>
@@ -6325,7 +6404,7 @@
       <c r="O3" s="28"/>
       <c r="P3" s="32"/>
       <c r="Q3" s="33" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="R3" s="28"/>
       <c r="S3" s="28"/>
@@ -6334,7 +6413,7 @@
       <c r="V3" s="28"/>
       <c r="W3" s="34"/>
       <c r="X3" s="35" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="Y3" s="28"/>
       <c r="Z3" s="36"/>
@@ -6359,12 +6438,12 @@
     </row>
     <row r="4" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
       <c r="H4" s="28"/>
       <c r="I4" s="28"/>
       <c r="J4" s="28"/>
@@ -6382,7 +6461,7 @@
       <c r="V4" s="28"/>
       <c r="W4" s="37"/>
       <c r="X4" s="38" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="Y4" s="28"/>
       <c r="Z4" s="36"/>
@@ -6408,7 +6487,7 @@
     <row r="5" spans="1:116" ht="23.25" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A5" s="3"/>
       <c r="B5" s="39" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C5" s="40"/>
       <c r="D5" s="40"/>
@@ -6425,7 +6504,7 @@
       <c r="O5" s="28"/>
       <c r="P5" s="41"/>
       <c r="Q5" s="33" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="R5" s="28"/>
       <c r="S5" s="28"/>
@@ -6434,7 +6513,7 @@
       <c r="V5" s="28"/>
       <c r="W5" s="42"/>
       <c r="X5" s="38" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="Y5" s="28"/>
       <c r="Z5" s="43"/>
@@ -6601,23 +6680,23 @@
     </row>
     <row r="9" spans="1:116" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="80" t="s">
+      <c r="B9" s="79" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="80" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="81" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="81" t="s">
+      <c r="G9" s="80" t="s">
         <v>89</v>
-      </c>
-      <c r="D9" s="82" t="s">
-        <v>90</v>
-      </c>
-      <c r="E9" s="81" t="s">
-        <v>91</v>
-      </c>
-      <c r="F9" s="82" t="s">
-        <v>92</v>
-      </c>
-      <c r="G9" s="81" t="s">
-        <v>93</v>
       </c>
       <c r="H9" s="49"/>
       <c r="I9" s="49"/>
@@ -6659,15 +6738,15 @@
     </row>
     <row r="10" spans="1:116" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="80"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="80"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
       <c r="H10" s="49"/>
       <c r="I10" s="49" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J10" s="49"/>
       <c r="K10" s="28"/>
@@ -7078,7 +7157,7 @@
     <row r="12" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="53" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C12" s="54">
         <v>1</v>
@@ -7208,7 +7287,7 @@
     <row r="13" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="53" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C13" s="54">
         <v>4</v>
@@ -7338,7 +7417,7 @@
     <row r="14" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="53" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C14" s="54"/>
       <c r="D14" s="55"/>
@@ -7458,7 +7537,7 @@
     <row r="15" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="53" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C15" s="54"/>
       <c r="D15" s="55"/>
@@ -7578,7 +7657,7 @@
     <row r="16" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="53" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C16" s="54"/>
       <c r="D16" s="55"/>
@@ -7698,7 +7777,7 @@
     <row r="17" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="53" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C17" s="54"/>
       <c r="D17" s="55"/>
@@ -7818,7 +7897,7 @@
     <row r="18" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="53" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C18" s="54"/>
       <c r="D18" s="55"/>
@@ -7938,7 +8017,7 @@
     <row r="19" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="53" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C19" s="54"/>
       <c r="D19" s="55"/>
@@ -8058,7 +8137,7 @@
     <row r="20" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="53" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C20" s="54"/>
       <c r="D20" s="55"/>
@@ -8178,7 +8257,7 @@
     <row r="21" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="53" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C21" s="54"/>
       <c r="D21" s="55"/>
@@ -8298,7 +8377,7 @@
     <row r="22" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="53" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C22" s="54"/>
       <c r="D22" s="55"/>
@@ -8418,7 +8497,7 @@
     <row r="23" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="53" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C23" s="54"/>
       <c r="D23" s="55"/>
@@ -8538,7 +8617,7 @@
     <row r="24" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="53" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C24" s="54"/>
       <c r="D24" s="55"/>
@@ -8658,7 +8737,7 @@
     <row r="25" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="53" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C25" s="54"/>
       <c r="D25" s="55"/>
@@ -8778,7 +8857,7 @@
     <row r="26" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="53" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C26" s="54"/>
       <c r="D26" s="55"/>
@@ -8898,7 +8977,7 @@
     <row r="27" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="53" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C27" s="54"/>
       <c r="D27" s="55"/>
@@ -9018,7 +9097,7 @@
     <row r="28" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="53" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C28" s="54"/>
       <c r="D28" s="55"/>
@@ -9138,7 +9217,7 @@
     <row r="29" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="53" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C29" s="54"/>
       <c r="D29" s="55"/>
@@ -9258,7 +9337,7 @@
     <row r="30" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="53" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C30" s="54"/>
       <c r="D30" s="55"/>
@@ -9378,7 +9457,7 @@
     <row r="31" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="53" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C31" s="54"/>
       <c r="D31" s="55"/>
@@ -9498,7 +9577,7 @@
     <row r="32" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="53" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C32" s="54"/>
       <c r="D32" s="55"/>
@@ -9618,7 +9697,7 @@
     <row r="33" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="53" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C33" s="54"/>
       <c r="D33" s="55"/>
@@ -9738,7 +9817,7 @@
     <row r="34" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="53" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C34" s="54"/>
       <c r="D34" s="55"/>
@@ -9858,7 +9937,7 @@
     <row r="35" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="53" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C35" s="54"/>
       <c r="D35" s="55"/>
@@ -9978,7 +10057,7 @@
     <row r="36" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="53" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C36" s="54"/>
       <c r="D36" s="55"/>
@@ -10098,7 +10177,7 @@
     <row r="37" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="53" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C37" s="54"/>
       <c r="D37" s="55"/>

</xml_diff>